<commit_message>
added computer to cost
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>Component</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>PDF link</t>
+  </si>
+  <si>
+    <t>75k Estimate</t>
+  </si>
+  <si>
+    <t>100k Estimate</t>
   </si>
 </sst>
 </file>
@@ -59,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +92,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,7 +136,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -146,6 +160,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -452,7 +467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
@@ -469,57 +484,114 @@
     <col min="7" max="7" width="15" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C1" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D3" s="2">
         <v>0.5</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E3" s="7">
         <v>5400</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G3" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C15" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="7">
+        <v>5400</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G17" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edited Cost for GPS
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>Component</t>
   </si>
@@ -56,6 +56,42 @@
   </si>
   <si>
     <t>100k Estimate</t>
+  </si>
+  <si>
+    <t>GPS Receiver</t>
+  </si>
+  <si>
+    <t>OEM 615</t>
+  </si>
+  <si>
+    <t>Novatel</t>
+  </si>
+  <si>
+    <t>1W</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Read GPS data and calculate Positon</t>
+  </si>
+  <si>
+    <t>GPS Antenna</t>
+  </si>
+  <si>
+    <t>Single Frequency Mircostrip</t>
+  </si>
+  <si>
+    <t>Antdevco</t>
+  </si>
+  <si>
+    <t>Recieves GPS and passes Signal to GPS</t>
+  </si>
+  <si>
+    <t>ANT-GPS</t>
+  </si>
+  <si>
+    <t>SpaceQuest</t>
   </si>
 </sst>
 </file>
@@ -223,7 +259,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -258,7 +294,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -467,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,6 +571,52 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="8">
+        <v>3000</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C15" s="9" t="s">
         <v>13</v>
@@ -583,6 +665,52 @@
         <v>9</v>
       </c>
       <c r="G17" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="8">
+        <v>5000</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -590,8 +718,12 @@
   <hyperlinks>
     <hyperlink ref="G17" r:id="rId1"/>
     <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G18" r:id="rId4"/>
+    <hyperlink ref="G19" r:id="rId5"/>
+    <hyperlink ref="G5" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added power data sheets and filled in excel sheet info
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
   <si>
     <t>Component</t>
   </si>
@@ -92,6 +92,33 @@
   </si>
   <si>
     <t>SpaceQuest</t>
+  </si>
+  <si>
+    <t>Recharge Battery and Power CubeSat</t>
+  </si>
+  <si>
+    <t>Manage Power for CubeSat</t>
+  </si>
+  <si>
+    <t>Power CubeSate (1 Battery)</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>NanoPower BPX</t>
+  </si>
+  <si>
+    <t>P31us</t>
+  </si>
+  <si>
+    <t>Power Management</t>
+  </si>
+  <si>
+    <t>Solar Panels</t>
+  </si>
+  <si>
+    <t>NanoPower P110</t>
   </si>
 </sst>
 </file>
@@ -205,6 +232,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -221,7 +316,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="424C3E"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -503,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,6 +712,75 @@
         <v>11</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="8">
+        <v>27000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>18</v>
+      </c>
+      <c r="E7" s="8">
+        <v>6200</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>0.115</v>
+      </c>
+      <c r="E8" s="8">
+        <v>6200</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C15" s="9" t="s">
         <v>13</v>
@@ -711,6 +875,75 @@
         <v>23</v>
       </c>
       <c r="G19" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="8">
+        <v>27000</v>
+      </c>
+      <c r="F20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21">
+        <v>18</v>
+      </c>
+      <c r="E21" s="8">
+        <v>6200</v>
+      </c>
+      <c r="F21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>0.115</v>
+      </c>
+      <c r="E22" s="8">
+        <v>6200</v>
+      </c>
+      <c r="F22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -722,8 +955,14 @@
     <hyperlink ref="G18" r:id="rId4"/>
     <hyperlink ref="G19" r:id="rId5"/>
     <hyperlink ref="G5" r:id="rId6"/>
+    <hyperlink ref="G6" r:id="rId7"/>
+    <hyperlink ref="G7" r:id="rId8"/>
+    <hyperlink ref="G8" r:id="rId9"/>
+    <hyperlink ref="G20" r:id="rId10"/>
+    <hyperlink ref="G21" r:id="rId11"/>
+    <hyperlink ref="G22" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Cost sheet, please review before I send it in.
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="63">
   <si>
     <t>Component</t>
   </si>
@@ -134,13 +134,83 @@
   </si>
   <si>
     <t>Power CubeSat (1 Battery)</t>
+  </si>
+  <si>
+    <t>MM2-TTL</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>FreeWave</t>
+  </si>
+  <si>
+    <t>4W (transmit)</t>
+  </si>
+  <si>
+    <t>Send Data to Ground Network</t>
+  </si>
+  <si>
+    <t>Antenna (Patch)</t>
+  </si>
+  <si>
+    <t>CS-CPUT-STX-02</t>
+  </si>
+  <si>
+    <t>ClydeSpace</t>
+  </si>
+  <si>
+    <t>2W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable Long distance Radio </t>
+  </si>
+  <si>
+    <t>Send Data to Ground Network w/ Dev kit</t>
+  </si>
+  <si>
+    <t>Attitude Control*</t>
+  </si>
+  <si>
+    <t>ISIS Magnetorqer Board</t>
+  </si>
+  <si>
+    <t>CubeSatShop</t>
+  </si>
+  <si>
+    <t>.175 - 1.2W</t>
+  </si>
+  <si>
+    <t>Provides Attitude Control</t>
+  </si>
+  <si>
+    <t>* Denotes additional hardware if Passive attitude does not allow for adequate sun sourced power</t>
+  </si>
+  <si>
+    <t>SP-L-DD1S3U-0039</t>
+  </si>
+  <si>
+    <t>Provides additional solar energy</t>
+  </si>
+  <si>
+    <t>Deployable Solar Panels*</t>
+  </si>
+  <si>
+    <t>Sun sensors (coarse)</t>
+  </si>
+  <si>
+    <t>integrated w/ solar panels</t>
+  </si>
+  <si>
+    <t>Price upcharge unkown for "fine" sensors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
@@ -214,7 +284,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -245,6 +315,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -552,15 +629,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="22.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="13" style="5" customWidth="1"/>
@@ -608,7 +685,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E3" s="6">
         <v>5400</v>
@@ -668,10 +745,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
@@ -679,22 +756,17 @@
       <c r="D6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="6">
-        <v>27000</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
@@ -703,10 +775,10 @@
         <v>17</v>
       </c>
       <c r="E7" s="6">
-        <v>6200</v>
+        <v>27000</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>11</v>
@@ -714,22 +786,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="5">
-        <v>0.3</v>
+      <c r="D8" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="E8" s="6">
         <v>6200</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>11</v>
@@ -737,28 +809,97 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="6">
+        <v>6200</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1000</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="6">
+        <v>4725</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E12" s="13">
         <v>0</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E12" s="6">
-        <f>SUM(E3:E11)</f>
-        <v>47800</v>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="12">
+        <f>SUM(E3:E12)</f>
+        <v>53525</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -800,7 +941,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E17" s="6">
         <v>5400</v>
@@ -860,10 +1001,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
@@ -871,22 +1012,17 @@
       <c r="D20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="6">
-        <v>27000</v>
-      </c>
       <c r="F20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
@@ -895,10 +1031,10 @@
         <v>17</v>
       </c>
       <c r="E21" s="6">
-        <v>6200</v>
+        <v>27000</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>11</v>
@@ -906,22 +1042,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="5">
-        <v>0.3</v>
+      <c r="D22" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="E22" s="6">
         <v>6200</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>11</v>
@@ -929,29 +1065,164 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="6">
+        <v>6200</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="6">
+        <v>1500</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="6">
+        <v>4725</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="6">
+        <v>19500</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E28" s="13">
         <v>0</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E27" s="6">
-        <f>SUM(E17:E22)</f>
-        <v>49800</v>
-      </c>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="12">
+        <f>SUM(E17:E28)</f>
+        <v>85525</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36" s="11"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -961,14 +1232,19 @@
     <hyperlink ref="G18" r:id="rId4"/>
     <hyperlink ref="G19" r:id="rId5"/>
     <hyperlink ref="G5" r:id="rId6"/>
-    <hyperlink ref="G6" r:id="rId7"/>
-    <hyperlink ref="G7" r:id="rId8"/>
-    <hyperlink ref="G8" r:id="rId9"/>
-    <hyperlink ref="G20" r:id="rId10"/>
-    <hyperlink ref="G21" r:id="rId11"/>
-    <hyperlink ref="G22" r:id="rId12"/>
+    <hyperlink ref="G7" r:id="rId7"/>
+    <hyperlink ref="G8" r:id="rId8"/>
+    <hyperlink ref="G9" r:id="rId9"/>
+    <hyperlink ref="G21" r:id="rId10"/>
+    <hyperlink ref="G22" r:id="rId11"/>
+    <hyperlink ref="G23" r:id="rId12"/>
+    <hyperlink ref="G10" r:id="rId13"/>
+    <hyperlink ref="G25" r:id="rId14"/>
+    <hyperlink ref="G11" r:id="rId15"/>
+    <hyperlink ref="G26" r:id="rId16"/>
+    <hyperlink ref="G27" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>